<commit_message>
Updating files in the Tahoe/Excel git repo Added a few new key files that are irreplacable, and updated files already in the repo
 Changes to be committed:
	new file:   CalibratingRMLands_Aug2014.xlsx
	modified:   Crosswalks/Condition Class Crosswalk 031513.xlsx
	modified:   Crosswalks/EVeg Classifications 5-22-2013.xlsx
	new file:   FRI and Percent Mortality Analysis.xlsx
	new file:   FRI possibilities.xlsx
	new file:   RMLands_Parameterization 082414.xlsx
	new file:   TahoeFireparams (version 1).xlsx
</commit_message>
<xml_diff>
--- a/Crosswalks/Condition Class Crosswalk 031513.xlsx
+++ b/Crosswalks/Condition Class Crosswalk 031513.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21520" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23540" windowHeight="15480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Crosswalk" sheetId="1" r:id="rId1"/>
@@ -881,7 +881,7 @@
   <dimension ref="A2:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -1055,7 +1055,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="16" customHeight="1">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1538,7 +1538,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>